<commit_message>
Add request skill trade
</commit_message>
<xml_diff>
--- a/AdvancedTask_NUnit/Manual Test/User Story 1 Manual Test.xlsx
+++ b/AdvancedTask_NUnit/Manual Test/User Story 1 Manual Test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="83">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -253,39 +253,31 @@
   </si>
   <si>
     <t>2. Change your earn target to "$1000 per month."</t>
+  </si>
+  <si>
+    <t>Verify that user can   "Send Requests for skill trade" .</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1. Click on the "Search Skills" button 2. Input user name in Search user then click.3.Click on the skill which you want to Trade with user.4.Click on Send Reguests button.</t>
+  </si>
+  <si>
+    <t>2.The "ReceivedRequests message  should be present on the user page.</t>
+  </si>
+  <si>
+    <t>TC18</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9.6"/>
-      <color rgb="FF374151"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9.6"/>
-      <color rgb="FF374151"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -309,23 +301,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF7F7F8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -343,79 +324,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFD9D9E3"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FFD9D9E3"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFD9D9E3"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFD9D9E3"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFD9D9E3"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFD9D9E3"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFD9D9E3"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFD9D9E3"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFD9D9E3"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFD9D9E3"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFD9D9E3"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFD9D9E3"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -434,45 +348,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="4" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
-    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
-    <cellStyle name="Good" xfId="2" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
+  <cellStyles count="4">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="4" builtinId="10"/>
+    <cellStyle name="Note" xfId="3" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -771,10 +666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,28 +682,28 @@
     <col min="7" max="7" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:8" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
@@ -821,21 +716,21 @@
       <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -844,16 +739,16 @@
       <c r="D3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="9"/>
-    </row>
-    <row r="4" spans="1:8" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G3" s="4"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>15</v>
       </c>
@@ -866,20 +761,20 @@
       <c r="D4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="9"/>
-    </row>
-    <row r="5" spans="1:8" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G4" s="4"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -888,16 +783,16 @@
       <c r="D5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="4" t="s">
         <v>78</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="9"/>
-    </row>
-    <row r="6" spans="1:8" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G5" s="4"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -916,10 +811,10 @@
       <c r="F6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="9"/>
-    </row>
-    <row r="7" spans="1:8" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G6" s="4"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>25</v>
       </c>
@@ -938,9 +833,9 @@
       <c r="F7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="5"/>
-    </row>
-    <row r="8" spans="1:8" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>29</v>
       </c>
@@ -959,9 +854,9 @@
       <c r="F8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="5"/>
-    </row>
-    <row r="9" spans="1:8" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>34</v>
       </c>
@@ -974,16 +869,16 @@
       <c r="D9" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="10"/>
-    </row>
-    <row r="10" spans="1:8" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G9" s="4"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>39</v>
       </c>
@@ -1002,24 +897,24 @@
       <c r="F10" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G10" s="5"/>
-    </row>
-    <row r="11" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6" t="s">
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-    </row>
-    <row r="12" spans="1:8" ht="44.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="4" t="s">
         <v>43</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -1028,14 +923,14 @@
       <c r="D12" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="4" t="s">
         <v>45</v>
       </c>
       <c r="F12" s="4"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="11"/>
-    </row>
-    <row r="13" spans="1:8" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G12" s="4"/>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>69</v>
       </c>
@@ -1052,9 +947,9 @@
         <v>48</v>
       </c>
       <c r="F13" s="4"/>
-      <c r="G13" s="5"/>
-    </row>
-    <row r="14" spans="1:8" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>70</v>
       </c>
@@ -1073,9 +968,9 @@
       <c r="F14" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G14" s="5"/>
-    </row>
-    <row r="15" spans="1:8" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>71</v>
       </c>
@@ -1094,9 +989,9 @@
       <c r="F15" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="G15" s="5"/>
-    </row>
-    <row r="16" spans="1:8" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>72</v>
       </c>
@@ -1113,9 +1008,9 @@
         <v>58</v>
       </c>
       <c r="F16" s="4"/>
-      <c r="G16" s="5"/>
-    </row>
-    <row r="17" spans="1:7" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>73</v>
       </c>
@@ -1132,9 +1027,9 @@
         <v>61</v>
       </c>
       <c r="F17" s="4"/>
-      <c r="G17" s="5"/>
-    </row>
-    <row r="18" spans="1:7" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>74</v>
       </c>
@@ -1151,9 +1046,9 @@
         <v>64</v>
       </c>
       <c r="F18" s="4"/>
-      <c r="G18" s="5"/>
-    </row>
-    <row r="19" spans="1:7" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>75</v>
       </c>
@@ -1172,7 +1067,26 @@
       <c r="F19" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="G19" s="1"/>
+      <c r="G19" s="4"/>
+    </row>
+    <row r="20" spans="1:7" ht="135.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>